<commit_message>
adding popups and new variable
</commit_message>
<xml_diff>
--- a/backend/data/climatologias_TEMPS.xlsx
+++ b/backend/data/climatologias_TEMPS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tmed" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tmean" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tmax" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Tmin" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -191,7 +191,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -957,7 +957,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>